<commit_message>
new version for create usergroup function & run the function after upload excel file
</commit_message>
<xml_diff>
--- a/uploads/Data.xlsx
+++ b/uploads/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10RS6N\Desktop\Node-API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F22316C-69B5-43ED-8349-42C0AD051DB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5081F48B-77D5-4DC2-A500-1AE04F831714}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>First Name</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>V5555</t>
+  </si>
+  <si>
+    <t>G5555</t>
   </si>
 </sst>
 </file>
@@ -545,7 +548,7 @@
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E6" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
update upload file path name
</commit_message>
<xml_diff>
--- a/uploads/Data.xlsx
+++ b/uploads/Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10RS6N\Desktop\Node-API\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10RS6N\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5081F48B-77D5-4DC2-A500-1AE04F831714}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E584DD5-92AE-4898-9268-25034599A596}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -102,7 +102,7 @@
     <t>V5555</t>
   </si>
   <si>
-    <t>G5555</t>
+    <t>G555</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
last updated version needs review
</commit_message>
<xml_diff>
--- a/uploads/Data.xlsx
+++ b/uploads/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10RS6N\Desktop\Node-API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76224E4-FC5C-4224-B115-2D860085979B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C58BA59-6A62-4769-8898-5E8152C7DA10}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4530" yWindow="30" windowWidth="9840" windowHeight="9450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>First Name</t>
   </si>
@@ -79,15 +79,6 @@
   </si>
   <si>
     <t>Hi</t>
-  </si>
-  <si>
-    <t>Action</t>
-  </si>
-  <si>
-    <t>+</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>zz11</t>
@@ -437,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E1" sqref="E1:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,7 +442,7 @@
     <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -464,11 +455,8 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -479,13 +467,10 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -496,13 +481,10 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -513,13 +495,10 @@
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -528,13 +507,10 @@
       </c>
       <c r="C5" s="2"/>
       <c r="D5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -545,10 +521,7 @@
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>